<commit_message>
letzter Stand vom 06.12.2016
letzter Stand vom 06.12.2016
</commit_message>
<xml_diff>
--- a/results/Datasets_infos.xlsx
+++ b/results/Datasets_infos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Glass</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Ann Thyroid</t>
+  </si>
+  <si>
+    <t>noch nicht mit GMD durchgelaufen</t>
   </si>
 </sst>
 </file>
@@ -393,18 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -418,7 +422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -433,17 +437,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>393</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">C3-1</f>
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>768</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -454,11 +481,11 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <f>C5-1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -469,11 +496,11 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <f>C6-1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -484,16 +511,29 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <f>C7-1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>330</v>
+      </c>
+      <c r="C8">
+        <v>501</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -504,11 +544,11 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <f>C9-1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -519,7 +559,7 @@
         <v>20</v>
       </c>
       <c r="D10">
-        <f>C10-1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>

</xml_diff>